<commit_message>
updated wellbeing reg files
</commit_message>
<xml_diff>
--- a/input/reg_wellbeing.xlsx
+++ b/input/reg_wellbeing.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{0E0ABAC9-582B-47C8-8A27-6E528F15610F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13128" windowHeight="6108" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UK_DWB_MCS1" sheetId="1" r:id="rId1"/>
@@ -159,7 +158,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -486,14 +485,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A25" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -594,7 +593,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -695,7 +694,7 @@
         <v>-1.9723185230582601E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -796,7 +795,7 @@
         <v>1.3836329181586601E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -897,7 +896,7 @@
         <v>-1.13840152293203E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -998,7 +997,7 @@
         <v>-1.0677004733819E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1099,7 +1098,7 @@
         <v>2.18686566012677E-6</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1200,7 +1199,7 @@
         <v>-1.01978799024498E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1301,7 +1300,7 @@
         <v>8.2335292115976103E-7</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1402,7 +1401,7 @@
         <v>-1.00174897709327E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1503,7 +1502,7 @@
         <v>-4.7544781176313903E-6</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1604,7 +1603,7 @@
         <v>-4.9584102760973099E-6</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1705,7 +1704,7 @@
         <v>-2.1505967285745799E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1806,7 +1805,7 @@
         <v>7.7656685937334398E-6</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1907,7 +1906,7 @@
         <v>-1.3213652434241101E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -2008,7 +2007,7 @@
         <v>-1.17086417374829E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -2109,7 +2108,7 @@
         <v>-1.5994575232654701E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -2210,7 +2209,7 @@
         <v>-6.0273609124951701E-6</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2311,7 +2310,7 @@
         <v>1.9126692962329499E-5</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2412,7 +2411,7 @@
         <v>2.79838915641631E-5</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -2513,7 +2512,7 @@
         <v>-3.3565124295039499E-6</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -2614,7 +2613,7 @@
         <v>2.7335548228489102E-6</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -2715,7 +2714,7 @@
         <v>1.1907039003452901E-5</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -2816,7 +2815,7 @@
         <v>2.34870277935497E-6</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2917,7 +2916,7 @@
         <v>-1.02300963338851E-5</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -3018,7 +3017,7 @@
         <v>-1.1855125027186299E-6</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -3119,7 +3118,7 @@
         <v>-4.3406424137561998E-7</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -3220,7 +3219,7 @@
         <v>5.8653743479097396E-6</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -3321,7 +3320,7 @@
         <v>-2.2221399140973902E-6</v>
       </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -3422,7 +3421,7 @@
         <v>5.3189045498413903E-9</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -3523,7 +3522,7 @@
         <v>1.0087059950724999E-5</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -3624,7 +3623,7 @@
         <v>3.1108388733936799E-5</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -3732,14 +3731,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3771,15 +3770,15 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2">
-        <v>-1.23806789329217</v>
+        <v>-1.23056636431974</v>
       </c>
       <c r="C2">
-        <v>0.100317399280766</v>
+        <v>0.103445250024589</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -3803,18 +3802,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="B3">
-        <v>1.38780817937347</v>
+        <v>1.4441139064634101</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>6.2452422154303203E-2</v>
+        <v>6.6087181550199103E-2</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -3835,12 +3834,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
       <c r="B4">
-        <v>-0.49963604315453097</v>
+        <v>-0.58348744071858405</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -3849,7 +3848,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>2.9542474928700799E-2</v>
+        <v>3.2081096346227099E-2</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -3867,12 +3866,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
       <c r="B5">
-        <v>-0.51154713626928605</v>
+        <v>-0.25042214934580498</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -3884,7 +3883,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>3.40532914727543E-2</v>
+        <v>4.6389313542080403E-2</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -3899,12 +3898,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>38</v>
       </c>
       <c r="B6">
-        <v>-0.78101737192389997</v>
+        <v>-0.86343025909766202</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -3919,7 +3918,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>4.2664867152636801E-2</v>
+        <v>6.3548920856129704E-2</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -3931,12 +3930,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>39</v>
       </c>
       <c r="B7">
-        <v>-1.0503607552260401</v>
+        <v>-1.0891121745363399</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -3954,7 +3953,7 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>4.4191386752414699E-2</v>
+        <v>6.8177272558643906E-2</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -3963,12 +3962,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>40</v>
       </c>
       <c r="B8">
-        <v>4.5693204959426303E-2</v>
+        <v>2.5702068477583499E-2</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -3989,18 +3988,18 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>1.1409961826623899E-2</v>
+        <v>1.5105874110923199E-2</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>41</v>
       </c>
       <c r="B9">
-        <v>-5.7247904366527297E-2</v>
+        <v>-0.16470758086589499</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -4024,7 +4023,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>8.12906050160302E-3</v>
+        <v>1.1374621686648E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4034,14 +4033,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4073,15 +4072,15 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2">
-        <v>-1.3489837784547301</v>
+        <v>-1.4228190123050499</v>
       </c>
       <c r="C2">
-        <v>0.17928898418012101</v>
+        <v>0.209206184901087</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -4105,18 +4104,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="B3">
-        <v>0.98956760678125599</v>
+        <v>1.0307197943903601</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>8.2726005601726105E-2</v>
+        <v>9.4849755363602295E-2</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -4137,12 +4136,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
       <c r="B4">
-        <v>-1.43604891505004</v>
+        <v>-1.3672336758516399</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -4151,7 +4150,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.100404428441737</v>
+        <v>0.117003284367741</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -4169,12 +4168,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
       <c r="B5">
-        <v>-0.47926807711235803</v>
+        <v>-0.46015958776090499</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -4186,7 +4185,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>4.9184064925410401E-2</v>
+        <v>7.2503426898626294E-2</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -4201,12 +4200,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>38</v>
       </c>
       <c r="B6">
-        <v>-0.80900137986986498</v>
+        <v>-0.70629664050724295</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -4221,7 +4220,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>6.0931848179205599E-2</v>
+        <v>9.82289801979849E-2</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -4233,12 +4232,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>39</v>
       </c>
       <c r="B7">
-        <v>-1.15688027451275</v>
+        <v>-1.2474728694726001</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -4256,7 +4255,7 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>7.4210585629514506E-2</v>
+        <v>0.12303306255009799</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -4265,12 +4264,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>40</v>
       </c>
       <c r="B8">
-        <v>4.85504102712042E-2</v>
+        <v>-9.5896950946945704E-3</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -4291,18 +4290,18 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>1.11826572333184E-2</v>
+        <v>1.57236914292413E-2</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>41</v>
       </c>
       <c r="B9">
-        <v>-0.114053804257953</v>
+        <v>-0.20401663530286501</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -4326,7 +4325,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>9.0062602331598893E-3</v>
+        <v>1.33149079995976E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4336,14 +4335,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4444,7 +4443,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -4545,7 +4544,7 @@
         <v>-3.22353089562766E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -4646,7 +4645,7 @@
         <v>6.51136105938806E-6</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -4747,7 +4746,7 @@
         <v>-3.30841592971335E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -4848,7 +4847,7 @@
         <v>-1.28898419618566E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -4949,7 +4948,7 @@
         <v>4.6837978312524999E-6</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -5050,7 +5049,7 @@
         <v>-4.3895321905892801E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -5151,7 +5150,7 @@
         <v>-2.6877392186348401E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -5252,7 +5251,7 @@
         <v>4.1651721326816596E-6</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -5353,7 +5352,7 @@
         <v>1.1598103721003699E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -5454,7 +5453,7 @@
         <v>-4.9879597895279201E-7</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -5555,7 +5554,7 @@
         <v>1.75634573887513E-6</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -5656,7 +5655,7 @@
         <v>3.0893105458824701E-6</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -5757,7 +5756,7 @@
         <v>1.06853589173559E-6</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -5858,7 +5857,7 @@
         <v>9.0893521624009207E-6</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -5959,7 +5958,7 @@
         <v>-5.5335189416960701E-6</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -6060,7 +6059,7 @@
         <v>1.12778457131741E-6</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -6161,7 +6160,7 @@
         <v>4.6632850064481498E-6</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -6262,7 +6261,7 @@
         <v>2.2734437963314201E-5</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -6363,7 +6362,7 @@
         <v>2.8917822788941702E-6</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -6464,7 +6463,7 @@
         <v>2.3349501290151199E-6</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -6565,7 +6564,7 @@
         <v>4.7055002298796301E-6</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -6666,7 +6665,7 @@
         <v>4.16440754957529E-6</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -6767,7 +6766,7 @@
         <v>-2.52036125994811E-5</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -6868,7 +6867,7 @@
         <v>1.68543195022551E-7</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -6969,7 +6968,7 @@
         <v>-4.88902804158497E-8</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -7070,7 +7069,7 @@
         <v>3.7696942795328101E-7</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -7171,7 +7170,7 @@
         <v>1.5919460882134401E-6</v>
       </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -7272,7 +7271,7 @@
         <v>-2.76987864498321E-8</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -7373,7 +7372,7 @@
         <v>6.1789356308933404E-6</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -7474,7 +7473,7 @@
         <v>3.5831306169954898E-5</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -7582,14 +7581,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7621,15 +7620,15 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2">
-        <v>0.138867401324514</v>
+        <v>0.14473670251260101</v>
       </c>
       <c r="C2">
-        <v>5.9835053773966598E-2</v>
+        <v>6.1273226234816798E-2</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -7653,18 +7652,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="B3">
-        <v>0.76773466344977703</v>
+        <v>0.72398980017675996</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>4.3234095266133601E-2</v>
+        <v>4.2677456089765899E-2</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -7685,12 +7684,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
       <c r="B4">
-        <v>-0.444053796232038</v>
+        <v>-0.40805728765892602</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -7699,7 +7698,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>2.4933085982321499E-2</v>
+        <v>2.5804704114682799E-2</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -7717,12 +7716,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
       <c r="B5">
-        <v>-0.53680560242889996</v>
+        <v>-0.64786512215603698</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -7734,7 +7733,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>3.1293859954548101E-2</v>
+        <v>3.7210638363925901E-2</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -7749,12 +7748,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>38</v>
       </c>
       <c r="B6">
-        <v>-0.626136313856266</v>
+        <v>-0.52790238319098104</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -7769,7 +7768,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>4.5297832724010799E-2</v>
+        <v>5.2968602686544401E-2</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -7781,12 +7780,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>39</v>
       </c>
       <c r="B7">
-        <v>-0.27959805032469298</v>
+        <v>-0.71118265552130999</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -7804,7 +7803,7 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>4.5463153788865E-2</v>
+        <v>5.4453392923858999E-2</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -7813,12 +7812,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>40</v>
       </c>
       <c r="B8">
-        <v>-0.12219813346464201</v>
+        <v>3.5313846726256898E-2</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -7839,18 +7838,18 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>1.09087261565764E-2</v>
+        <v>1.0665778176003801E-2</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>41</v>
       </c>
       <c r="B9">
-        <v>0.122167871893469</v>
+        <v>0.14230834922964999</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -7874,7 +7873,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>7.1106471538351403E-3</v>
+        <v>8.1244931188861596E-3</v>
       </c>
     </row>
   </sheetData>
@@ -7884,14 +7883,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7923,15 +7922,15 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2">
-        <v>1.13375308945563</v>
+        <v>0.96700780202930603</v>
       </c>
       <c r="C2">
-        <v>0.108453698235043</v>
+        <v>0.11319861709536</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -7955,18 +7954,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="B3">
-        <v>-0.12216290847771701</v>
+        <v>-8.7236005864526206E-2</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>6.7465493336152996E-2</v>
+        <v>7.3896310888152197E-2</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -7987,12 +7986,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
       <c r="B4">
-        <v>-0.25508933358576602</v>
+        <v>-0.32979624167820298</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -8001,7 +8000,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>7.1338870659180403E-2</v>
+        <v>7.8297133540976296E-2</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -8019,12 +8018,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
       <c r="B5">
-        <v>-0.74865421560811196</v>
+        <v>-0.72965074119122597</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -8036,7 +8035,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>4.3817315585549403E-2</v>
+        <v>5.8308252125873698E-2</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -8051,12 +8050,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>38</v>
       </c>
       <c r="B6">
-        <v>-1.19885571142589</v>
+        <v>-0.70814708182476604</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -8071,7 +8070,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>6.1501350904321697E-2</v>
+        <v>7.6068346940108E-2</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -8083,12 +8082,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>39</v>
       </c>
       <c r="B7">
-        <v>-1.1583925593992901</v>
+        <v>-1.0288942592311801</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -8106,7 +8105,7 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>6.3807604004587903E-2</v>
+        <v>8.2842310652720505E-2</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -8115,12 +8114,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>40</v>
       </c>
       <c r="B8">
-        <v>-0.102258528057334</v>
+        <v>-9.5008964591471401E-2</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -8141,18 +8140,18 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>8.5802608911340703E-3</v>
+        <v>9.8134737056849008E-3</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>41</v>
       </c>
       <c r="B9">
-        <v>8.6042401206758198E-2</v>
+        <v>6.1434528696179998E-2</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -8176,7 +8175,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>7.136880693175E-3</v>
+        <v>8.7577694998627904E-3</v>
       </c>
     </row>
   </sheetData>
@@ -8186,14 +8185,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8297,7 +8296,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -8401,7 +8400,7 @@
         <v>-4.9277747548168296E-6</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -8505,7 +8504,7 @@
         <v>2.4678602856380201E-7</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -8609,7 +8608,7 @@
         <v>-6.5780876088898396E-8</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -8713,7 +8712,7 @@
         <v>-3.9446657144982999E-7</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -8817,7 +8816,7 @@
         <v>7.2184138280628094E-8</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -8921,7 +8920,7 @@
         <v>-1.9765901244502201E-7</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -9025,7 +9024,7 @@
         <v>5.4735423894817602E-8</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -9129,7 +9128,7 @@
         <v>-2.9529291982246602E-7</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -9233,7 +9232,7 @@
         <v>-9.9060284980097005E-8</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -9337,7 +9336,7 @@
         <v>-6.1534999529330898E-8</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -9441,7 +9440,7 @@
         <v>-2.5297241829426502E-7</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -9545,7 +9544,7 @@
         <v>-2.6561260173068902E-7</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -9649,7 +9648,7 @@
         <v>1.75939406341646E-8</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -9753,7 +9752,7 @@
         <v>-8.15533656720696E-8</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -9857,7 +9856,7 @@
         <v>-2.7506839597320802E-7</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -9961,7 +9960,7 @@
         <v>1.51972853559985E-7</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -10065,7 +10064,7 @@
         <v>-6.8918506693187602E-8</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -10169,7 +10168,7 @@
         <v>-8.9374874272991503E-8</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -10273,7 +10272,7 @@
         <v>-2.1146652760150401E-7</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -10377,7 +10376,7 @@
         <v>-2.1193024614442699E-7</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -10481,7 +10480,7 @@
         <v>-7.7047851803442506E-8</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -10585,7 +10584,7 @@
         <v>-1.2572114713105301E-7</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -10689,7 +10688,7 @@
         <v>1.9354481235019499E-8</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -10793,7 +10792,7 @@
         <v>-7.0566310812153796E-8</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -10897,7 +10896,7 @@
         <v>-1.21044477417085E-8</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -11001,7 +11000,7 @@
         <v>-1.21850168715562E-8</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -11105,7 +11104,7 @@
         <v>6.5177522631869098E-8</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -11209,7 +11208,7 @@
         <v>-1.66024769990004E-8</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -11313,7 +11312,7 @@
         <v>-1.3441718551676401E-10</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -11417,7 +11416,7 @@
         <v>3.0463769675704402E-7</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -11521,7 +11520,7 @@
         <v>7.5701423572371002E-7</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -11632,14 +11631,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11671,15 +11670,15 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2">
-        <v>-0.104268458083628</v>
+        <v>-9.9638023612954804E-2</v>
       </c>
       <c r="C2">
-        <v>2.08254814417314E-3</v>
+        <v>2.1877917000088401E-3</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -11703,18 +11702,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="B3">
-        <v>4.7545309147170402E-2</v>
+        <v>6.12046933064666E-2</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1.58509715165359E-3</v>
+        <v>1.7090782019972899E-3</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -11735,12 +11734,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
       <c r="B4">
-        <v>-8.4688919955804201E-2</v>
+        <v>-7.9217973407544703E-2</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -11749,7 +11748,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>6.9063192545085899E-4</v>
+        <v>7.6124667237600896E-4</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -11767,12 +11766,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
       <c r="B5">
-        <v>-0.14128788739527501</v>
+        <v>-0.13470996687658601</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -11784,7 +11783,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>8.4413164058314396E-4</v>
+        <v>1.2411083062172201E-3</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -11799,12 +11798,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>38</v>
       </c>
       <c r="B6">
-        <v>-8.01559142718066E-2</v>
+        <v>-0.115184567399258</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -11819,7 +11818,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>9.9302707671454992E-4</v>
+        <v>1.44347865994554E-3</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -11831,12 +11830,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>39</v>
       </c>
       <c r="B7">
-        <v>-0.114247431380457</v>
+        <v>-0.153507417191036</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -11854,7 +11853,7 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>9.7547237546313E-4</v>
+        <v>1.50291263094377E-3</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -11863,12 +11862,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>40</v>
       </c>
       <c r="B8">
-        <v>-9.07856479815272E-3</v>
+        <v>-1.21940132240634E-2</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -11889,18 +11888,18 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>2.72939551202962E-4</v>
+        <v>3.6956120195602002E-4</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>41</v>
       </c>
       <c r="B9">
-        <v>5.8837267400241597E-3</v>
+        <v>-1.61707100239993E-2</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -11924,7 +11923,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>1.8565230967818299E-4</v>
+        <v>2.5383801812351998E-4</v>
       </c>
     </row>
   </sheetData>
@@ -11934,14 +11933,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11973,15 +11972,15 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2">
-        <v>-0.24974629169884</v>
+        <v>-0.241099051541424</v>
       </c>
       <c r="C2">
-        <v>3.8820081237897499E-3</v>
+        <v>4.4857959823730101E-3</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -12005,18 +12004,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="B3">
-        <v>4.56278095398477E-2</v>
+        <v>7.2105821167758502E-2</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>2.71656409468029E-3</v>
+        <v>3.1340383658325301E-3</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -12037,12 +12036,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
       <c r="B4">
-        <v>-0.38000054772123099</v>
+        <v>-0.33578763811511397</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -12051,7 +12050,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>2.39672123854441E-3</v>
+        <v>2.6440006564389502E-3</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -12069,12 +12068,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
       <c r="B5">
-        <v>-0.14888778267656899</v>
+        <v>-0.141027262742555</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -12086,7 +12085,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>1.3126140535323599E-3</v>
+        <v>1.91969597551501E-3</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -12101,12 +12100,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>38</v>
       </c>
       <c r="B6">
-        <v>-0.19983324866302801</v>
+        <v>-0.185338761984772</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -12121,7 +12120,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>1.51746854789051E-3</v>
+        <v>2.2383139962641502E-3</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -12133,12 +12132,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>39</v>
       </c>
       <c r="B7">
-        <v>-0.16581620375849801</v>
+        <v>-0.172122215639476</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -12156,7 +12155,7 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>1.5492062011097901E-3</v>
+        <v>2.3839546743497902E-3</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -12165,12 +12164,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>40</v>
       </c>
       <c r="B8">
-        <v>5.79073777457837E-3</v>
+        <v>7.0854464583095999E-3</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -12191,18 +12190,18 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>2.9668717070747302E-4</v>
+        <v>3.9984848987148697E-4</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>41</v>
       </c>
       <c r="B9">
-        <v>-2.24770775051913E-2</v>
+        <v>-4.36990950739094E-2</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -12226,7 +12225,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>2.4672527979899901E-4</v>
+        <v>3.6007712287628498E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>